<commit_message>
Save 18 08 2025
</commit_message>
<xml_diff>
--- a/4 четверть_12_JavaScript_nodejs_Валидация данных.xlsx
+++ b/4 четверть_12_JavaScript_nodejs_Валидация данных.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9FBD92-FFB0-4E2F-B1FA-879E97508739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D7A075-4236-420F-A322-86BD05D71A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-480" yWindow="-15780" windowWidth="23010" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fastest validation" sheetId="14" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="379">
   <si>
     <t>Урок 1 часть 1</t>
   </si>
@@ -8861,17 +8861,37 @@
 }
 </t>
   </si>
+  <si>
+    <t xml:space="preserve">                const schema = {
+                    email: { 
+                        type: "email",
+                        messages: {
+                          email: "Пожалуйста, введите корректный email!"
+                        },
+                        normalize: true, // приводит email к lowercase
+                        empty: false, // запрещает пустую строку
+                    }
+                }</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -9101,9 +9121,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -9114,57 +9134,57 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -9173,7 +9193,7 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -9182,13 +9202,16 @@
     <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9475,10 +9498,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:V183"/>
+  <dimension ref="A2:V184"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A137" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11225,481 +11248,490 @@
       <c r="B143" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C143" s="21" t="s">
+      <c r="C143" s="31" t="s">
         <v>154</v>
       </c>
       <c r="D143" s="21" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A144" s="24" t="s">
+    <row r="144" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="B144" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C144" s="31" t="s">
+        <v>378</v>
+      </c>
+      <c r="D144" s="21"/>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="B145" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C144" s="21" t="s">
+      <c r="C145" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="D144" s="1" t="s">
+      <c r="D145" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A145" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B145" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C145" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D145" s="26"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B146" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C146" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D146" s="26"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="B146" s="26" t="s">
+      <c r="B147" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="C146" s="26" t="s">
+      <c r="C147" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="D146" s="26"/>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A147" s="27" t="s">
+      <c r="D147" s="26"/>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" s="27" t="s">
         <v>347</v>
       </c>
-      <c r="B147" s="27"/>
-      <c r="C147" s="27" t="s">
+      <c r="B148" s="27"/>
+      <c r="C148" s="27" t="s">
         <v>348</v>
       </c>
-      <c r="D147" s="27" t="s">
+      <c r="D148" s="27" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="B148" s="2" t="s">
+    <row r="149" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B149" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C148" s="21" t="s">
+      <c r="C149" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="D148" s="21" t="s">
+      <c r="D149" s="21" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A149" s="24" t="s">
+    <row r="150" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A150" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="B150" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C149" s="21" t="s">
+      <c r="C150" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="D149" s="1" t="s">
+      <c r="D150" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A150" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B150" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C150" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D150" s="26"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="26" t="s">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="B151" s="26" t="s">
-        <v>171</v>
+        <v>71</v>
       </c>
       <c r="C151" s="26" t="s">
-        <v>172</v>
+        <v>72</v>
       </c>
       <c r="D151" s="26"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B152" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="C152" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="D152" s="26"/>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="B152" s="26" t="s">
+      <c r="B153" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C152" s="26" t="s">
+      <c r="C153" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="D152" s="26"/>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A153" s="27" t="s">
+      <c r="D153" s="26"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154" s="27" t="s">
         <v>347</v>
       </c>
-      <c r="B153" s="27"/>
-      <c r="C153" s="27" t="s">
+      <c r="B154" s="27"/>
+      <c r="C154" s="27" t="s">
         <v>348</v>
       </c>
-      <c r="D153" s="27" t="s">
+      <c r="D154" s="27" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="144" x14ac:dyDescent="0.3">
-      <c r="A154" s="1" t="s">
+    <row r="155" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="A155" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="B155" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C154" s="21" t="s">
+      <c r="C155" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="D154" s="21" t="s">
+      <c r="D155" s="21" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A155" s="1" t="s">
+    <row r="156" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A156" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="B156" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C155" s="21" t="s">
+      <c r="C156" s="21" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A156" s="24" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="C156" s="21" t="s">
+      <c r="C157" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="D156" s="1" t="s">
+      <c r="D157" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A157" s="26" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B157" s="26" t="s">
+      <c r="B158" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C157" s="26" t="s">
+      <c r="C158" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D157" s="26"/>
-    </row>
-    <row r="158" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A158" s="26" t="s">
+      <c r="D158" s="26"/>
+    </row>
+    <row r="159" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A159" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="B158" s="26" t="s">
+      <c r="B159" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C158" s="26" t="s">
+      <c r="C159" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="D158" s="26"/>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A159" s="27" t="s">
+      <c r="D159" s="26"/>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A160" s="27" t="s">
         <v>347</v>
       </c>
-      <c r="B159" s="27"/>
-      <c r="C159" s="27" t="s">
+      <c r="B160" s="27"/>
+      <c r="C160" s="27" t="s">
         <v>348</v>
       </c>
-      <c r="D159" s="27" t="s">
+      <c r="D160" s="27" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B160" s="2" t="s">
+    <row r="161" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B161" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C160" s="21" t="s">
+      <c r="C161" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="D160" s="21" t="s">
+      <c r="D161" s="21" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A161" s="1" t="s">
+    <row r="162" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A162" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="B162" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C161" s="21" t="s">
+      <c r="C162" s="21" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A162" s="24" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A163" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="C162" s="21" t="s">
+      <c r="C163" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="D162" s="1" t="s">
+      <c r="D163" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A163" s="27" t="s">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A164" s="27" t="s">
         <v>347</v>
       </c>
-      <c r="B163" s="27"/>
-      <c r="C163" s="27" t="s">
+      <c r="B164" s="27"/>
+      <c r="C164" s="27" t="s">
         <v>348</v>
       </c>
-      <c r="D163" s="27" t="s">
+      <c r="D164" s="27" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B164" s="2" t="s">
+    <row r="165" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B165" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C164" s="21" t="s">
+      <c r="C165" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="D164" s="21" t="s">
+      <c r="D165" s="21" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A165" s="24" t="s">
+    <row r="166" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A166" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="B165" s="2" t="s">
+      <c r="B166" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C165" s="21" t="s">
+      <c r="C166" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="D165" s="1" t="s">
+      <c r="D166" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A166" s="27" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167" s="27" t="s">
         <v>347</v>
       </c>
-      <c r="B166" s="27"/>
-      <c r="C166" s="27" t="s">
+      <c r="B167" s="27"/>
+      <c r="C167" s="27" t="s">
         <v>348</v>
       </c>
-      <c r="D166" s="27" t="s">
+      <c r="D167" s="27" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B167" s="2" t="s">
+    <row r="168" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B168" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C167" s="21" t="s">
+      <c r="C168" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="D167" s="21" t="s">
+      <c r="D168" s="21" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A168" s="24" t="s">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A169" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="B168" s="2" t="s">
+      <c r="B169" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C168" s="21" t="s">
+      <c r="C169" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D168" s="1" t="s">
+      <c r="D169" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A169" s="27" t="s">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A170" s="27" t="s">
         <v>347</v>
       </c>
-      <c r="B169" s="27"/>
-      <c r="C169" s="27" t="s">
+      <c r="B170" s="27"/>
+      <c r="C170" s="27" t="s">
         <v>348</v>
       </c>
-      <c r="D169" s="27" t="s">
+      <c r="D170" s="27" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B170" s="2" t="s">
+    <row r="171" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B171" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C170" s="21" t="s">
+      <c r="C171" s="21" t="s">
         <v>313</v>
       </c>
-      <c r="D170" s="21" t="s">
+      <c r="D171" s="21" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A171" s="24" t="s">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A172" s="24" t="s">
         <v>308</v>
       </c>
-      <c r="C171" s="21" t="s">
+      <c r="C172" s="21" t="s">
         <v>309</v>
       </c>
-      <c r="D171" s="1" t="s">
+      <c r="D172" s="1" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A172" s="27" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A173" s="27" t="s">
         <v>347</v>
       </c>
-      <c r="B172" s="27"/>
-      <c r="C172" s="27" t="s">
+      <c r="B173" s="27"/>
+      <c r="C173" s="27" t="s">
         <v>348</v>
       </c>
-      <c r="D172" s="27" t="s">
+      <c r="D173" s="27" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B173" s="2" t="s">
+    <row r="174" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B174" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C173" s="2" t="s">
+      <c r="C174" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D173" s="2" t="s">
+      <c r="D174" s="2" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A174" s="24" t="s">
+    <row r="175" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A175" s="24" t="s">
         <v>314</v>
       </c>
-      <c r="C174" s="21" t="s">
+      <c r="C175" s="21" t="s">
         <v>315</v>
       </c>
-      <c r="D174" s="21" t="s">
+      <c r="D175" s="21" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A175" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B175" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C175" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D175" s="26"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B176" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C176" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D176" s="26"/>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A177" s="26" t="s">
         <v>317</v>
       </c>
-      <c r="B176" s="26" t="s">
+      <c r="B177" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="C176" s="26" t="s">
+      <c r="C177" s="26" t="s">
         <v>318</v>
       </c>
-      <c r="D176" s="26"/>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A177" s="27" t="s">
+      <c r="D177" s="26"/>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A178" s="27" t="s">
         <v>347</v>
       </c>
-      <c r="B177" s="27"/>
-      <c r="C177" s="27" t="s">
+      <c r="B178" s="27"/>
+      <c r="C178" s="27" t="s">
         <v>348</v>
       </c>
-      <c r="D177" s="27" t="s">
+      <c r="D178" s="27" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="144" x14ac:dyDescent="0.3">
-      <c r="B178" s="2" t="s">
+    <row r="179" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="B179" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C178" s="21" t="s">
+      <c r="C179" s="21" t="s">
         <v>328</v>
       </c>
-      <c r="D178" s="21" t="s">
+      <c r="D179" s="21" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A179" s="24" t="s">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A180" s="24" t="s">
         <v>319</v>
       </c>
-      <c r="C179" s="21" t="s">
+      <c r="C180" s="21" t="s">
         <v>320</v>
       </c>
-      <c r="D179" s="1" t="s">
+      <c r="D180" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A180" s="26" t="s">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A181" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B180" s="26" t="s">
+      <c r="B181" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C180" s="26" t="s">
+      <c r="C181" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D180" s="26"/>
-    </row>
-    <row r="181" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A181" s="26" t="s">
+      <c r="D181" s="26"/>
+    </row>
+    <row r="182" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A182" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="B181" s="26" t="s">
+      <c r="B182" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C181" s="26" t="s">
+      <c r="C182" s="26" t="s">
         <v>324</v>
       </c>
-      <c r="D181" s="26"/>
-    </row>
-    <row r="182" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B182" s="2" t="s">
+      <c r="D182" s="26"/>
+    </row>
+    <row r="183" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B183" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C182" s="21" t="s">
+      <c r="C183" s="21" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A183" s="21" t="s">
+    <row r="184" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A184" s="21" t="s">
         <v>327</v>
       </c>
-      <c r="B183" s="2" t="s">
+      <c r="B184" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C183" s="21" t="s">
+      <c r="C184" s="21" t="s">
         <v>325</v>
       </c>
     </row>
@@ -12097,7 +12129,7 @@
       <c r="V3" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
save 22 08 2025
</commit_message>
<xml_diff>
--- a/4 четверть_12_JavaScript_nodejs_Валидация данных.xlsx
+++ b/4 четверть_12_JavaScript_nodejs_Валидация данных.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D7A075-4236-420F-A322-86BD05D71A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE49BFC-1C55-4F4A-BF58-FA0E66D4F20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13875" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fastest validation" sheetId="14" r:id="rId1"/>
@@ -31,12 +31,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="384">
   <si>
     <t>Урок 1 часть 1</t>
   </si>
@@ -6372,106 +6375,6 @@
 */</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">const schema = {
-    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>username</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: { 
-        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: "string", 
-        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>min</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: 3, trim: true, 
-        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>lowercase</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: true
-    }
-}
-</t>
-    </r>
-  </si>
-  <si>
     <t>`https://github.com/icebob/fastest-validator?tab=readme-ov-file#record</t>
   </si>
   <si>
@@ -7183,13 +7086,6 @@
     <t>Shorthand definitions</t>
   </si>
   <si>
-    <t>const schema = {
-    password: "string|min:6",
-    age: "number|optional|integer|positive|min:0|max:99", // additional properties
-    state: ["boolean", "number|min:0|max:1"] // multiple types
-}</t>
-  </si>
-  <si>
     <t>You can use string-based shorthand validation definitions in the schema.</t>
   </si>
   <si>
@@ -7221,22 +7117,6 @@
   </si>
   <si>
     <t>The most common sanitizer is the default property. With it, you can define a default value for all properties. If the property value is null* or undefined, the validator set the defined default value into the property.</t>
-  </si>
-  <si>
-    <t>const schema = {
-    roles: { type: "array", items: "string", default: ["user"] },
-    status: { type: "boolean", default: true },
-};
-const check = v.compile(schema);
-const obj = {}
-check(obj); // Valid
-console.log(obj);
-/*
-{
-    roles: ["user"],
-    status: true
-}
-*/</t>
   </si>
   <si>
     <r>
@@ -8838,12 +8718,6 @@
 check({}); // Fail because undefined is disallowed</t>
   </si>
   <si>
-    <t xml:space="preserve">const schema = {
-    age: { type: "number", nullable: true }
-}
-</t>
-  </si>
-  <si>
     <t>Strict validation</t>
   </si>
   <si>
@@ -8853,13 +8727,6 @@
     <t>const check = v.compile(schema);
 check({ name: "John" }); // Valid
 check({ name: "John", age: 42 }); // Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">const schema = {
-    name: { type: "string" }, // required
-    $$strict: true // no additional properties allowed
-}
-</t>
   </si>
   <si>
     <t xml:space="preserve">                const schema = {
@@ -8873,17 +8740,575 @@
                     }
                 }</t>
   </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>front</t>
+  </si>
+  <si>
+    <r>
+      <t>removeEmailFromAllSendouts(){
+                let emailTrimmed = this.inputFilterPlaning.trim();
+                this.emailIsCorrect = this.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>checkUserInputIsCorrectEmail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(emailTrimmed) === true ? true : false;
+                if(this.emailIsCorrect){
+                    this.$confirm(`Вы действительно хотите удалить ${emailTrimmed} из всех рассылок и шаблонов?`, "", {
+                      confirmButtonText: 'Да',
+                      cancelButtonText: 'Нет',
+                      type: 'warning'
+                    }).then(() =&gt; {
+                        this.$http.post('/api/manage/removeEmailFromAllSendouts', {
+                            UserMail: emailTrimmed
+                        }).then(result =&gt; {
+                            this.$message({
+                                message: `Операция выполнена: ${emailTrimmed} успешно удалён из всех рассылок и шаблонов`,
+                                type: 'info'
+                            });
+                        }). catch(err =&gt; {
+                            this.$message({
+                                message: `Операция провалена: ${emailTrimmed} не удалён из рассылок и шаблонов`,
+                                type: 'error'
+                            });
+                        })
+                    }).catch(() =&gt; {
+                    });
+                }</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>checkUserInputIsCorrectEmail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(email){
+                let res = false;
+                </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>const v = new Validator();
+                const schema = {
+                    email: { 
+                        type: "email",
+                        normalize: true,
+                        empty: false,
+                    }
+                }</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+                const checkInputIsEmail = v.compile(schema);
+                res = !Array.isArray(checkInputIsEmail({ email }))
+                return res;
+            },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">const schema = {
+    roles: { type: "array", items: "string", </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>default: ["user"]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> },
+    status: { type: "boolean",</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> default: true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> },
+};
+const check = v.compile(schema);
+const obj = {}
+check(obj); // Valid
+console.log(obj);
+/*
+{
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>roles: ["user"],
+    status: true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+}
+*/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">const schema = {
+    password: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"string|min:6"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,
+    age: "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>number|optional|integer|positive|min:0|max:99</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">", // additional properties
+    state: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>["boolean", "number|min:0|max:1"]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> // multiple types
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">const schema = {
+    age: { type: "number", </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nullable: true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> }
+}
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">const schema = {
+    name: { type: "string" }, // required
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> $$strict: true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> // no additional properties allowed
+}
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">const schema = {
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>username</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: { 
+        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: "string", 
+        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>min</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 3, 
+        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>trim</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: true, 
+        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lowercase</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: true
+    }
+}
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">const schema = {
+    password: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"string|min:6"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,
+    age: {
+        type: "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">number",
+        optional: true, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//age field can be omited inside the object</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+        integer: true,
+        positive: true,
+        min: 0,
+        max: 99</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,
+    }
+}</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -9047,8 +9472,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -9109,6 +9541,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -9121,9 +9559,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -9134,57 +9572,57 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -9193,7 +9631,7 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -9202,13 +9640,19 @@
     <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -9498,10 +9942,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:V184"/>
+  <dimension ref="A2:V188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C143" sqref="C143"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9555,223 +9999,174 @@
       <c r="U2" s="5"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>365</v>
+      <c r="A3" s="32" t="s">
+        <v>374</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="U3" s="5"/>
-    </row>
-    <row r="4" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>367</v>
+      <c r="G3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="U3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>377</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="U4" s="5"/>
-    </row>
-    <row r="5" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+      <c r="G4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="1:22" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
-        <v>368</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="U5" s="5"/>
-    </row>
-    <row r="6" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>375</v>
-      </c>
+      <c r="G5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="U6" s="5"/>
-    </row>
-    <row r="7" spans="1:22" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>377</v>
-      </c>
+      <c r="G6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="U6" s="1"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
+        <v>362</v>
+      </c>
+      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="U7" s="5"/>
+      <c r="G7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="U7" s="1"/>
     </row>
     <row r="8" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="U8" s="5"/>
-    </row>
-    <row r="9" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="G8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="1:22" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="G9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="G10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="U9" s="5"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
-        <v>330</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="P10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="2"/>
-    </row>
-    <row r="11" spans="1:22" ht="72" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="G11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="G12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="G13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="23" t="s">
+        <v>329</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="P11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="2"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
-        <v>334</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="P12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="2"/>
-    </row>
-    <row r="13" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C13" s="21" t="s">
-        <v>335</v>
-      </c>
-      <c r="P13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="2"/>
-    </row>
-    <row r="14" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>338</v>
       </c>
       <c r="P14" s="1"/>
       <c r="U14" s="1"/>
       <c r="V14" s="2"/>
     </row>
-    <row r="15" spans="1:22" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>341</v>
-      </c>
+    <row r="15" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>339</v>
+        <v>330</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>379</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>383</v>
       </c>
       <c r="P15" s="1"/>
       <c r="U15" s="1"/>
@@ -9779,1960 +10174,2005 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="s">
+        <v>332</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="P16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="2"/>
+    </row>
+    <row r="17" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C17" s="21" t="s">
+        <v>333</v>
+      </c>
+      <c r="P17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="2"/>
+    </row>
+    <row r="18" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>378</v>
+      </c>
+      <c r="P18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="2"/>
+    </row>
+    <row r="19" spans="1:22" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>336</v>
+      </c>
+      <c r="P19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="2"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A20" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C20" s="22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="24" t="s">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A21" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C21" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
+    <row r="22" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C22" s="21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="24" t="s">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A23" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C23" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="25" t="s">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A24" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B24" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C24" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="27"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="25" t="s">
+      <c r="D24" s="27"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A25" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B25" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C25" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="27"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="25" t="s">
+      <c r="D25" s="27"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A26" s="25" t="s">
         <v>76</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="27"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="27"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="27"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="D25" s="27"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="25" t="s">
-        <v>85</v>
       </c>
       <c r="B26" s="26" t="s">
         <v>77</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D26" s="27"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B27" s="26" t="s">
         <v>77</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D27" s="27"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="25" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B28" s="26" t="s">
         <v>77</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D28" s="27"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="25" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B29" s="26" t="s">
         <v>77</v>
       </c>
       <c r="C29" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="27"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A30" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="27"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A31" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="27"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A32" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="27"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="27"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="21" t="s">
+      <c r="D33" s="27"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C35" s="21" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="21" t="s">
+    <row r="36" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C36" s="21" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="21" t="s">
+    <row r="37" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C37" s="21" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="21" t="s">
+    <row r="38" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C38" s="21" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="21" t="s">
+    <row r="39" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C39" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="24" t="s">
+    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="C40" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="D40" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="D36" s="1" t="s">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" s="26"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D42" s="26"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="C43" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="D43" s="26"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="21"/>
+      <c r="B45" s="2" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="26" t="s">
+      <c r="C45" s="21" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="21"/>
+      <c r="B46" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="21"/>
+      <c r="B47" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B50" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C50" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D37" s="26"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="26"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" s="26" t="s">
-        <v>171</v>
-      </c>
-      <c r="C39" s="26" t="s">
-        <v>303</v>
-      </c>
-      <c r="D39" s="26"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D40" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="21"/>
-      <c r="B41" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="21"/>
-      <c r="B42" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="21"/>
-      <c r="B43" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="C43" s="21" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="24" t="s">
-        <v>226</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="25" t="s">
+      <c r="D50" s="25"/>
+    </row>
+    <row r="51" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A51" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="D51" s="25"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="D52" s="25"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="D53" s="25"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B54" s="27"/>
+      <c r="C54" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D54" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="360" x14ac:dyDescent="0.3">
+      <c r="A55" s="21"/>
+      <c r="B55" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A56" s="21"/>
+      <c r="B56" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="21"/>
+      <c r="B57" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C58" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="25" t="s">
+      <c r="B59" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="25" t="s">
+      <c r="C59" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D46" s="25"/>
-    </row>
-    <row r="47" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A47" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="B47" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" s="29" t="s">
-        <v>235</v>
-      </c>
-      <c r="D47" s="25"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="B48" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C48" s="25" t="s">
-        <v>231</v>
-      </c>
-      <c r="D48" s="25"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="B49" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C49" s="25" t="s">
-        <v>233</v>
-      </c>
-      <c r="D49" s="25"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B50" s="27"/>
-      <c r="C50" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D50" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="360" x14ac:dyDescent="0.3">
-      <c r="A51" s="21"/>
-      <c r="B51" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="302.39999999999998" x14ac:dyDescent="0.3">
-      <c r="A52" s="21"/>
-      <c r="B52" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="C52" s="21" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="21"/>
-      <c r="B53" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="C53" s="21" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="24" t="s">
+      <c r="D59" s="26"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="26" t="s">
         <v>292</v>
       </c>
-      <c r="C54" s="21" t="s">
-        <v>291</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B55" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C55" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D55" s="26"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="26" t="s">
+      <c r="B60" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="C60" s="26" t="s">
         <v>293</v>
       </c>
-      <c r="B56" s="26" t="s">
-        <v>240</v>
-      </c>
-      <c r="C56" s="26" t="s">
+      <c r="D60" s="26"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C61" s="26" t="s">
         <v>294</v>
       </c>
-      <c r="D56" s="26"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="B57" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C57" s="26" t="s">
+      <c r="D61" s="26"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B62" s="27"/>
+      <c r="C62" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D62" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="B63" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="D57" s="26"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B58" s="27"/>
-      <c r="C58" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D58" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="B59" s="2" t="s">
+      <c r="C63" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="C59" s="21" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="24" t="s">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C60" s="21"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B61" s="27"/>
-      <c r="C61" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D61" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="288" x14ac:dyDescent="0.3">
-      <c r="A62" s="21" t="s">
+      <c r="C64" s="21"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B65" s="27"/>
+      <c r="C65" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D65" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="288" x14ac:dyDescent="0.3">
+      <c r="A66" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C62" s="21" t="s">
+      <c r="C66" s="21" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="24" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="C63" s="21" t="s">
+      <c r="C67" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B64" s="27"/>
-      <c r="C64" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D64" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="216" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B68" s="27"/>
+      <c r="C68" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D68" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C65" s="21" t="s">
+      <c r="C69" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="B66" s="2" t="s">
+      <c r="D69" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="B70" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C70" s="21" t="s">
+        <v>340</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="C66" s="21" t="s">
+    </row>
+    <row r="71" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C71" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C67" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="24" t="s">
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="C68" s="21" t="s">
+      <c r="C72" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D72" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="B69" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C69" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="D69" s="27"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B70" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C70" s="27" t="s">
-        <v>213</v>
-      </c>
-      <c r="D70" s="27"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B71" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C71" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="D71" s="27"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="B72" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C72" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="D72" s="27"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="27" t="s">
-        <v>216</v>
+        <v>70</v>
       </c>
       <c r="B73" s="27" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C73" s="27" t="s">
-        <v>217</v>
+        <v>72</v>
       </c>
       <c r="D73" s="27"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="27" t="s">
-        <v>218</v>
+        <v>76</v>
       </c>
       <c r="B74" s="27" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="C74" s="27" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D74" s="27"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="27" t="s">
-        <v>220</v>
+        <v>79</v>
       </c>
       <c r="B75" s="27" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="C75" s="27" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D75" s="27"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="27" t="s">
-        <v>222</v>
+        <v>162</v>
       </c>
       <c r="B76" s="27" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="C76" s="27" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D76" s="27"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="27" t="s">
-        <v>91</v>
+        <v>216</v>
       </c>
       <c r="B77" s="27" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="C77" s="27" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D77" s="27"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B78" s="27"/>
+        <v>218</v>
+      </c>
+      <c r="B78" s="27" t="s">
+        <v>97</v>
+      </c>
       <c r="C78" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D78" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A79" s="2"/>
-      <c r="B79" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C79" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="D79" s="21" t="s">
-        <v>350</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="D78" s="27"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="B79" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C79" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="D79" s="27"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>284</v>
-      </c>
+      <c r="A80" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="B80" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C80" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="D80" s="27"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="27" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="B81" s="27" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="C81" s="27" t="s">
-        <v>72</v>
+        <v>224</v>
       </c>
       <c r="D81" s="27"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="B82" s="27" t="s">
-        <v>74</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="B82" s="27"/>
       <c r="C82" s="27" t="s">
-        <v>241</v>
-      </c>
-      <c r="D82" s="27"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B83" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C83" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="D83" s="27"/>
+        <v>345</v>
+      </c>
+      <c r="D82" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C83" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="D83" s="21" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B84" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C84" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="D84" s="27"/>
+      <c r="A84" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="27" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C85" s="27" t="s">
-        <v>242</v>
+        <v>72</v>
       </c>
       <c r="D85" s="27"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="27" t="s">
-        <v>243</v>
+        <v>73</v>
       </c>
       <c r="B86" s="27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C86" s="27" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D86" s="27"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="27" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B87" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C87" s="27" t="s">
-        <v>245</v>
+        <v>150</v>
       </c>
       <c r="D87" s="27"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="27" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B88" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C88" s="27" t="s">
-        <v>246</v>
+        <v>151</v>
       </c>
       <c r="D88" s="27"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="27" t="s">
-        <v>247</v>
+        <v>81</v>
       </c>
       <c r="B89" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C89" s="27" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D89" s="27"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="27" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B90" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C90" s="27" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D90" s="27"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="27" t="s">
-        <v>251</v>
+        <v>83</v>
       </c>
       <c r="B91" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C91" s="27" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="D91" s="27"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="27" t="s">
-        <v>253</v>
+        <v>87</v>
       </c>
       <c r="B92" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C92" s="27" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="D92" s="27"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="27" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="B93" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C93" s="27" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D93" s="27"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="27" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="B94" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C94" s="27" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="D94" s="27"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="27" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="B95" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C95" s="27" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="D95" s="27"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="27" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B96" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C96" s="27" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="D96" s="27"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="27" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="B97" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C97" s="27" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="D97" s="27"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="27" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B98" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C98" s="27" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="D98" s="27"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="27" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B99" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C99" s="27" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="D99" s="27"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="27" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B100" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C100" s="27" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="D100" s="27"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="27" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="B101" s="27" t="s">
-        <v>272</v>
+        <v>77</v>
       </c>
       <c r="C101" s="27" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="D101" s="27"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="27" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="B102" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C102" s="27" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="D102" s="27"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="27" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B103" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C103" s="27" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="D103" s="27"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="27" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="B104" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C104" s="27" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="D104" s="27"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="27" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B105" s="27" t="s">
-        <v>77</v>
+        <v>272</v>
       </c>
       <c r="C105" s="27" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="D105" s="27"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="27" t="s">
-        <v>91</v>
+        <v>274</v>
       </c>
       <c r="B106" s="27" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="C106" s="27" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D106" s="27"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B107" s="27"/>
+        <v>276</v>
+      </c>
+      <c r="B107" s="27" t="s">
+        <v>77</v>
+      </c>
       <c r="C107" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D107" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A108" s="2"/>
-      <c r="B108" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="B109" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>287</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="D107" s="27"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="27" t="s">
+        <v>278</v>
+      </c>
+      <c r="B108" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C108" s="27" t="s">
+        <v>279</v>
+      </c>
+      <c r="D108" s="27"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="B109" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C109" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="D109" s="27"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C110" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="A110" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B110" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C110" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="D110" s="27"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B111" s="27"/>
+      <c r="C111" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D111" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A112" s="2"/>
+      <c r="B112" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="B113" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C114" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="B111" s="26" t="s">
+      <c r="B115" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C111" s="28" t="s">
+      <c r="C115" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="D111" s="27"/>
-    </row>
-    <row r="112" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A112" s="27" t="s">
+      <c r="D115" s="27"/>
+    </row>
+    <row r="116" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A116" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="B112" s="26" t="s">
+      <c r="B116" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C112" s="28" t="s">
+      <c r="C116" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="D112" s="27"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B113" s="27"/>
-      <c r="C113" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D113" s="27" t="s">
+      <c r="D116" s="27"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B117" s="27"/>
+      <c r="C117" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D117" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B118" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C118" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D118" s="21" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B114" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C114" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="D114" s="21" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="B115" s="2" t="s">
+    <row r="119" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B119" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C119" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D119" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" s="24" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="B116" s="1"/>
-      <c r="C116" s="1" t="s">
+      <c r="B120" s="1"/>
+      <c r="C120" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D120" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="26" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B117" s="26" t="s">
+      <c r="B121" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C117" s="26" t="s">
+      <c r="C121" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D117" s="26"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="B118" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C118" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="D118" s="26"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B119" s="27"/>
-      <c r="C119" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D119" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="B120" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C120" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="D120" s="21" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C121" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>115</v>
-      </c>
+      <c r="D121" s="26"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="26" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="B122" s="26" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C122" s="26" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="D122" s="26"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="B123" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C123" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="D123" s="26"/>
-    </row>
-    <row r="124" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A124" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="B124" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="C124" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D124" s="26"/>
+      <c r="A123" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B123" s="27"/>
+      <c r="C123" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D123" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B124" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C124" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="D124" s="21" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="B125" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="C125" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D125" s="26"/>
+      <c r="A125" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C125" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="26" t="s">
-        <v>124</v>
+        <v>70</v>
       </c>
       <c r="B126" s="26" t="s">
-        <v>125</v>
+        <v>71</v>
       </c>
       <c r="C126" s="26" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="D126" s="26"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="26" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B127" s="26" t="s">
         <v>77</v>
       </c>
       <c r="C127" s="26" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D127" s="26"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B128" s="27"/>
-      <c r="C128" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D128" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" ht="144" x14ac:dyDescent="0.3">
-      <c r="B129" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C129" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="D129" s="21" t="s">
-        <v>354</v>
-      </c>
+    <row r="128" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A128" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B128" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C128" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D128" s="26"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B129" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C129" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D129" s="26"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A130" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C130" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="A130" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B130" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C130" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D130" s="26"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="B131" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C131" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D131" s="26"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B132" s="27"/>
+      <c r="C132" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D132" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="B133" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C133" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="D133" s="21" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C134" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B131" s="26" t="s">
+      <c r="B135" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C131" s="26" t="s">
+      <c r="C135" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D131" s="26"/>
-    </row>
-    <row r="132" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A132" s="26" t="s">
+      <c r="D135" s="26"/>
+    </row>
+    <row r="136" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A136" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="B132" s="26" t="s">
+      <c r="B136" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C132" s="26" t="s">
+      <c r="C136" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="D132" s="26"/>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B133" s="27"/>
-      <c r="C133" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D133" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="B134" s="2" t="s">
+      <c r="D136" s="26"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B137" s="27"/>
+      <c r="C137" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D137" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B138" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C134" s="21" t="s">
+      <c r="C138" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D134" s="21" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" s="24" t="s">
+      <c r="D138" s="21" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B139" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C135" s="21" t="s">
+      <c r="C139" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="D135" s="1" t="s">
+      <c r="D139" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A136" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B136" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C136" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D136" s="26"/>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A137" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B137" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="C137" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="D137" s="26"/>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A138" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="B138" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="C138" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="D138" s="26"/>
-    </row>
-    <row r="139" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A139" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="B139" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="C139" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="D139" s="26"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="26" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B140" s="26" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C140" s="26" t="s">
-        <v>150</v>
+        <v>72</v>
       </c>
       <c r="D140" s="26"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B141" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C141" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="D141" s="26"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="B142" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="C142" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="D142" s="26"/>
+    </row>
+    <row r="143" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A143" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B143" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C143" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D143" s="26"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B144" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C144" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="D144" s="26"/>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="B141" s="26" t="s">
+      <c r="B145" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="C141" s="26" t="s">
+      <c r="C145" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="D141" s="26"/>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A142" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B142" s="27"/>
-      <c r="C142" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D142" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B143" s="2" t="s">
+      <c r="D145" s="26"/>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B146" s="27"/>
+      <c r="C146" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D146" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B147" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C143" s="31" t="s">
+      <c r="C147" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="D143" s="21" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" ht="144" x14ac:dyDescent="0.3">
-      <c r="B144" s="2" t="s">
+      <c r="D147" s="21" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="B148" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C144" s="31" t="s">
-        <v>378</v>
-      </c>
-      <c r="D144" s="21"/>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A145" s="24" t="s">
+      <c r="C148" s="31" t="s">
+        <v>373</v>
+      </c>
+      <c r="D148" s="21"/>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B149" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C145" s="21" t="s">
+      <c r="C149" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="D145" s="1" t="s">
+      <c r="D149" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A146" s="26" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B146" s="26" t="s">
+      <c r="B150" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C146" s="26" t="s">
+      <c r="C150" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D146" s="26"/>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A147" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="B147" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C147" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="D147" s="26"/>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A148" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B148" s="27"/>
-      <c r="C148" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D148" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="B149" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C149" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="D149" s="21" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A150" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C150" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="D150" s="26"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="B151" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C151" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="D151" s="26"/>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B152" s="27"/>
+      <c r="C152" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D152" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B153" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C153" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="D153" s="21" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A154" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C154" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B151" s="26" t="s">
+      <c r="B155" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C151" s="26" t="s">
+      <c r="C155" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D151" s="26"/>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A152" s="26" t="s">
+      <c r="D155" s="26"/>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="B152" s="26" t="s">
+      <c r="B156" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="C152" s="26" t="s">
+      <c r="C156" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="D152" s="26"/>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A153" s="26" t="s">
+      <c r="D156" s="26"/>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="B153" s="26" t="s">
+      <c r="B157" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C153" s="26" t="s">
+      <c r="C157" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="D153" s="26"/>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A154" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B154" s="27"/>
-      <c r="C154" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D154" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" ht="144" x14ac:dyDescent="0.3">
-      <c r="A155" s="1" t="s">
+      <c r="D157" s="26"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B158" s="27"/>
+      <c r="C158" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D158" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="A159" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="B159" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C155" s="21" t="s">
+      <c r="C159" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="D155" s="21" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A156" s="1" t="s">
+      <c r="D159" s="21" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A160" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="B160" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C156" s="21" t="s">
+      <c r="C160" s="21" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A157" s="24" t="s">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="C157" s="21" t="s">
+      <c r="C161" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="D157" s="1" t="s">
+      <c r="D161" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A158" s="26" t="s">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A162" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B158" s="26" t="s">
+      <c r="B162" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C158" s="26" t="s">
+      <c r="C162" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D158" s="26"/>
-    </row>
-    <row r="159" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A159" s="26" t="s">
+      <c r="D162" s="26"/>
+    </row>
+    <row r="163" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A163" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="B159" s="26" t="s">
+      <c r="B163" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C159" s="26" t="s">
+      <c r="C163" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="D159" s="26"/>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A160" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B160" s="27"/>
-      <c r="C160" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D160" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B161" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C161" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="D161" s="21" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A162" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C162" s="21" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A163" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="C163" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>190</v>
-      </c>
+      <c r="D163" s="26"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="27" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B164" s="27"/>
       <c r="C164" s="27" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D164" s="27" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B165" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C165" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="D165" s="21" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A166" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C166" s="21" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C167" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A168" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B168" s="27"/>
+      <c r="C168" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D168" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B169" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C165" s="21" t="s">
+      <c r="C169" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="D165" s="21" t="s">
+      <c r="D169" s="21" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A170" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C170" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A171" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B171" s="27"/>
+      <c r="C171" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D171" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B172" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C172" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="D172" s="21" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A173" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C173" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A174" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B174" s="27"/>
+      <c r="C174" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D174" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B175" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C175" s="21" t="s">
+        <v>312</v>
+      </c>
+      <c r="D175" s="21" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A176" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="C176" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A177" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D177" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B178" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D178" s="2" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A166" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C166" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="D166" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A167" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B167" s="27"/>
-      <c r="C167" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D167" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B168" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C168" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="D168" s="21" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A169" s="24" t="s">
-        <v>199</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C169" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A170" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B170" s="27"/>
-      <c r="C170" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D170" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B171" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C171" s="21" t="s">
+    <row r="179" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A179" s="24" t="s">
         <v>313</v>
       </c>
-      <c r="D171" s="21" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A172" s="24" t="s">
-        <v>308</v>
-      </c>
-      <c r="C172" s="21" t="s">
-        <v>309</v>
-      </c>
-      <c r="D172" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A173" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B173" s="27"/>
-      <c r="C173" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D173" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B174" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="C174" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="D174" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A175" s="24" t="s">
+      <c r="C179" s="21" t="s">
         <v>314</v>
       </c>
-      <c r="C175" s="21" t="s">
-        <v>315</v>
-      </c>
-      <c r="D175" s="21" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A176" s="26" t="s">
+      <c r="D179" s="21" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A180" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B176" s="26" t="s">
+      <c r="B180" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C176" s="26" t="s">
+      <c r="C180" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D176" s="26"/>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A177" s="26" t="s">
-        <v>317</v>
-      </c>
-      <c r="B177" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C177" s="26" t="s">
-        <v>318</v>
-      </c>
-      <c r="D177" s="26"/>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A178" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B178" s="27"/>
-      <c r="C178" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D178" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" ht="144" x14ac:dyDescent="0.3">
-      <c r="B179" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="C179" s="21" t="s">
-        <v>328</v>
-      </c>
-      <c r="D179" s="21" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A180" s="24" t="s">
-        <v>319</v>
-      </c>
-      <c r="C180" s="21" t="s">
-        <v>320</v>
-      </c>
-      <c r="D180" s="1" t="s">
-        <v>322</v>
-      </c>
+      <c r="D180" s="26"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="B181" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C181" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="D181" s="26"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A182" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="B182" s="27"/>
+      <c r="C182" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D182" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="B183" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C183" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="D183" s="21" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A184" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="C184" s="21" t="s">
+        <v>319</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A185" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B181" s="26" t="s">
+      <c r="B185" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C181" s="26" t="s">
+      <c r="C185" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D181" s="26"/>
-    </row>
-    <row r="182" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A182" s="26" t="s">
+      <c r="D185" s="26"/>
+    </row>
+    <row r="186" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A186" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="B182" s="26" t="s">
+      <c r="B186" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C182" s="26" t="s">
+      <c r="C186" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="D186" s="26"/>
+    </row>
+    <row r="187" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B187" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C187" s="21" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A188" s="21" t="s">
+        <v>326</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C188" s="21" t="s">
         <v>324</v>
-      </c>
-      <c r="D182" s="26"/>
-    </row>
-    <row r="183" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B183" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C183" s="21" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A184" s="21" t="s">
-        <v>327</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="C184" s="21" t="s">
-        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -12129,7 +12569,7 @@
       <c r="V3" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>